<commit_message>
Formatting update to Gantt
</commit_message>
<xml_diff>
--- a/Documents/Gantt Chart/Gantt_Weekly_Status1.xlsx
+++ b/Documents/Gantt Chart/Gantt_Weekly_Status1.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="22430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Satan\Documents\GitHub\Trajectory\Documents\Gantt Chart\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lucas Thoms\Desktop\Idaho\2020 1Spring\CS 383\Trajectory\Documents\Gantt Chart\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C3A973B-43B9-4E4D-8BC1-7C5D8A766A2A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E72607B4-75A4-4526-99C8-4ECB55860639}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{E656BF53-8C2F-9143-90A0-23AA440D0AB5}"/>
+    <workbookView xWindow="-103" yWindow="-103" windowWidth="21600" windowHeight="13869" xr2:uid="{E656BF53-8C2F-9143-90A0-23AA440D0AB5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -32,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="97">
   <si>
     <t>Task</t>
   </si>
@@ -73,9 +75,6 @@
     <t>Finalization</t>
   </si>
   <si>
-    <t>Lucas Thomas</t>
-  </si>
-  <si>
     <t>Understanding Requirements</t>
   </si>
   <si>
@@ -299,12 +298,42 @@
   </si>
   <si>
     <t>in Progress</t>
+  </si>
+  <si>
+    <t>Integrating MVP</t>
+  </si>
+  <si>
+    <t>Lucas Thoms</t>
+  </si>
+  <si>
+    <t>Total Cost</t>
+  </si>
+  <si>
+    <t>Jan 30th</t>
+  </si>
+  <si>
+    <t>Budget</t>
+  </si>
+  <si>
+    <t>Actual</t>
+  </si>
+  <si>
+    <t>Delta</t>
+  </si>
+  <si>
+    <t>Meetings</t>
+  </si>
+  <si>
+    <t>S</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
   <fonts count="5">
     <font>
       <sz val="12"/>
@@ -390,7 +419,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -398,11 +427,122 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="double">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
@@ -440,19 +580,63 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
@@ -768,25 +952,31 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F1596FC7-FBA9-FA4D-A1A3-B3A3B96D1437}">
-  <dimension ref="A1:BR84"/>
+  <dimension ref="A1:BR86"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="61" workbookViewId="0">
-      <selection activeCell="G43" sqref="G43"/>
+    <sheetView tabSelected="1" zoomScale="61" workbookViewId="0">
+      <selection activeCell="M81" sqref="M81"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.9"/>
+  <cols>
+    <col min="8" max="8" width="13.85546875" customWidth="1"/>
+    <col min="9" max="9" width="11.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="10.78515625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="12.140625" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:68">
-      <c r="A1" s="24" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="25"/>
-      <c r="C1" s="25"/>
-      <c r="D1" s="25"/>
-      <c r="E1" s="24" t="s">
-        <v>55</v>
-      </c>
-      <c r="F1" s="24"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="27" t="s">
+        <v>54</v>
+      </c>
+      <c r="F1" s="27"/>
       <c r="G1" s="1" t="s">
         <v>1</v>
       </c>
@@ -794,16 +984,16 @@
         <v>2</v>
       </c>
       <c r="I1" s="17" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J1" s="14" t="s">
+        <v>47</v>
+      </c>
+      <c r="K1" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>49</v>
-      </c>
       <c r="L1" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="2" spans="1:68">
@@ -999,12 +1189,12 @@
       </c>
     </row>
     <row r="3" spans="1:68">
-      <c r="A3" s="25" t="s">
+      <c r="A3" s="28" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="25"/>
-      <c r="C3" s="25"/>
-      <c r="D3" s="25"/>
+      <c r="B3" s="28"/>
+      <c r="C3" s="28"/>
+      <c r="D3" s="28"/>
       <c r="E3">
         <v>1</v>
       </c>
@@ -1015,17 +1205,17 @@
         <v>1</v>
       </c>
       <c r="H3" s="7" t="s">
-        <v>49</v>
-      </c>
-      <c r="I3" s="14"/>
+        <v>48</v>
+      </c>
+      <c r="I3" s="7"/>
     </row>
     <row r="4" spans="1:68">
-      <c r="A4" s="25" t="s">
+      <c r="A4" s="28" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="25"/>
-      <c r="C4" s="25"/>
-      <c r="D4" s="25"/>
+      <c r="B4" s="28"/>
+      <c r="C4" s="28"/>
+      <c r="D4" s="28"/>
       <c r="E4">
         <v>2</v>
       </c>
@@ -1036,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="H4" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J4" s="16">
         <v>1</v>
@@ -1058,12 +1248,12 @@
       <c r="Y4" s="10"/>
     </row>
     <row r="5" spans="1:68">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="25"/>
-      <c r="C5" s="25"/>
-      <c r="D5" s="25"/>
+      <c r="B5" s="28"/>
+      <c r="C5" s="28"/>
+      <c r="D5" s="28"/>
       <c r="E5">
         <v>3</v>
       </c>
@@ -1071,7 +1261,7 @@
         <v>5</v>
       </c>
       <c r="H5" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="J5" s="16">
         <v>1</v>
@@ -1082,12 +1272,12 @@
       <c r="N5" s="15"/>
     </row>
     <row r="6" spans="1:68">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="23"/>
-      <c r="C6" s="23"/>
-      <c r="D6" s="23"/>
+      <c r="B6" s="26"/>
+      <c r="C6" s="26"/>
+      <c r="D6" s="26"/>
       <c r="E6">
         <v>4</v>
       </c>
@@ -1095,7 +1285,7 @@
         <v>5</v>
       </c>
       <c r="H6" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O6" s="16">
         <v>3</v>
@@ -1106,12 +1296,12 @@
       <c r="S6" s="15"/>
     </row>
     <row r="7" spans="1:68">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="26" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="23"/>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
+      <c r="B7" s="26"/>
+      <c r="C7" s="26"/>
+      <c r="D7" s="26"/>
       <c r="E7">
         <v>5</v>
       </c>
@@ -1119,7 +1309,7 @@
         <v>4</v>
       </c>
       <c r="H7" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="T7" s="16">
         <v>4</v>
@@ -1129,12 +1319,12 @@
       <c r="W7" s="15"/>
     </row>
     <row r="8" spans="1:68">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="23"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
+      <c r="B8" s="26"/>
+      <c r="C8" s="26"/>
+      <c r="D8" s="26"/>
       <c r="E8">
         <v>6</v>
       </c>
@@ -1145,7 +1335,7 @@
         <v>1</v>
       </c>
       <c r="H8" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="X8" s="16">
         <v>5</v>
@@ -1153,12 +1343,12 @@
       <c r="Y8" s="15"/>
     </row>
     <row r="9" spans="1:68">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="26" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="23"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
+      <c r="B9" s="26"/>
+      <c r="C9" s="26"/>
+      <c r="D9" s="26"/>
       <c r="E9">
         <v>7</v>
       </c>
@@ -1167,20 +1357,20 @@
       </c>
       <c r="G9" s="13"/>
       <c r="H9" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z9" s="15" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="AA9" s="15"/>
     </row>
     <row r="10" spans="1:68">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="B10" s="23"/>
-      <c r="C10" s="23"/>
-      <c r="D10" s="23"/>
+      <c r="B10" s="26"/>
+      <c r="C10" s="26"/>
+      <c r="D10" s="26"/>
       <c r="E10">
         <v>8</v>
       </c>
@@ -1188,7 +1378,7 @@
         <v>5</v>
       </c>
       <c r="H10" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AB10" s="16">
         <v>7</v>
@@ -1199,12 +1389,12 @@
       <c r="AF10" s="15"/>
     </row>
     <row r="11" spans="1:68">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="26" t="s">
         <v>12</v>
       </c>
-      <c r="B11" s="23"/>
-      <c r="C11" s="23"/>
-      <c r="D11" s="23"/>
+      <c r="B11" s="26"/>
+      <c r="C11" s="26"/>
+      <c r="D11" s="26"/>
       <c r="E11">
         <v>9</v>
       </c>
@@ -1212,7 +1402,7 @@
         <v>3</v>
       </c>
       <c r="H11" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1225,28 +1415,28 @@
       <c r="AI11" s="16"/>
     </row>
     <row r="12" spans="1:68">
-      <c r="A12" s="26" t="s">
-        <v>50</v>
-      </c>
-      <c r="B12" s="26"/>
-      <c r="C12" s="26"/>
-      <c r="D12" s="26"/>
+      <c r="A12" s="24" t="s">
+        <v>49</v>
+      </c>
+      <c r="B12" s="24"/>
+      <c r="C12" s="24"/>
+      <c r="D12" s="24"/>
       <c r="E12" s="10"/>
       <c r="F12" s="10"/>
       <c r="G12">
         <v>2</v>
       </c>
       <c r="I12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="13" spans="1:68">
-      <c r="A13" s="23" t="s">
-        <v>25</v>
-      </c>
-      <c r="B13" s="23"/>
-      <c r="C13" s="23"/>
-      <c r="D13" s="23"/>
+      <c r="A13" s="26" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="26"/>
+      <c r="C13" s="26"/>
+      <c r="D13" s="26"/>
       <c r="F13">
         <f>SUM(F3:F11)</f>
         <v>28</v>
@@ -1258,7 +1448,7 @@
     </row>
     <row r="14" spans="1:68">
       <c r="A14" s="2" t="s">
-        <v>13</v>
+        <v>89</v>
       </c>
       <c r="B14" s="2"/>
       <c r="C14" s="2"/>
@@ -1322,7 +1512,7 @@
     </row>
     <row r="15" spans="1:68">
       <c r="A15" s="8" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" s="8"/>
       <c r="C15" s="8"/>
@@ -1337,7 +1527,7 @@
         <v>2</v>
       </c>
       <c r="H15" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I15" s="7"/>
       <c r="J15" s="7"/>
@@ -1346,7 +1536,7 @@
     </row>
     <row r="16" spans="1:68">
       <c r="A16" s="8" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" s="8"/>
       <c r="C16" s="8"/>
@@ -1358,19 +1548,19 @@
         <v>2</v>
       </c>
       <c r="G16">
-        <v>1</v>
-      </c>
-      <c r="H16" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I16" s="14"/>
-      <c r="J16" s="14"/>
+      <c r="I16" s="7"/>
+      <c r="J16" s="7"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
     </row>
     <row r="17" spans="1:70">
       <c r="A17" s="8" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" s="8"/>
       <c r="C17" s="8"/>
@@ -1382,19 +1572,19 @@
         <v>2</v>
       </c>
       <c r="G17">
-        <v>1</v>
-      </c>
-      <c r="H17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17" s="7" t="s">
         <v>48</v>
       </c>
-      <c r="I17" s="14"/>
-      <c r="J17" s="14"/>
+      <c r="I17" s="7"/>
+      <c r="J17" s="7"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
     </row>
     <row r="18" spans="1:70">
       <c r="A18" s="8" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" s="8"/>
       <c r="C18" s="8"/>
@@ -1406,15 +1596,15 @@
         <v>4</v>
       </c>
       <c r="G18">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="H18" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I18" s="13"/>
       <c r="J18" s="13"/>
       <c r="K18" s="14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="L18" s="14"/>
       <c r="M18" s="14"/>
@@ -1422,7 +1612,7 @@
     </row>
     <row r="19" spans="1:70">
       <c r="A19" s="8" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" s="8"/>
       <c r="C19" s="8"/>
@@ -1433,16 +1623,19 @@
       <c r="F19">
         <v>3</v>
       </c>
-      <c r="H19" s="12" t="s">
-        <v>52</v>
+      <c r="G19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="14" t="s">
+        <v>47</v>
       </c>
       <c r="M19" s="13"/>
       <c r="N19" s="13"/>
-      <c r="O19" s="16">
+      <c r="O19" s="19">
         <v>4</v>
       </c>
-      <c r="P19" s="15"/>
-      <c r="Q19" s="15"/>
+      <c r="P19" s="14"/>
+      <c r="Q19" s="14"/>
       <c r="R19" s="10"/>
       <c r="S19" s="10"/>
       <c r="T19" s="10"/>
@@ -1452,7 +1645,7 @@
     </row>
     <row r="20" spans="1:70">
       <c r="A20" s="8" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" s="8"/>
       <c r="C20" s="8"/>
@@ -1464,7 +1657,7 @@
         <v>3</v>
       </c>
       <c r="H20" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O20" s="16">
         <v>4</v>
@@ -1473,12 +1666,12 @@
       <c r="Q20" s="15"/>
     </row>
     <row r="21" spans="1:70">
-      <c r="A21" s="27" t="s">
-        <v>62</v>
-      </c>
-      <c r="B21" s="27"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
+      <c r="A21" s="25" t="s">
+        <v>61</v>
+      </c>
+      <c r="B21" s="25"/>
+      <c r="C21" s="25"/>
+      <c r="D21" s="25"/>
       <c r="E21">
         <v>7</v>
       </c>
@@ -1486,7 +1679,7 @@
         <v>6</v>
       </c>
       <c r="H21" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="R21" s="16">
         <v>6</v>
@@ -1499,7 +1692,7 @@
     </row>
     <row r="22" spans="1:70">
       <c r="A22" s="8" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B22" s="8"/>
       <c r="C22" s="8"/>
@@ -1511,10 +1704,10 @@
         <v>6</v>
       </c>
       <c r="H22" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="X22" s="15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="Y22" s="15"/>
       <c r="Z22" s="15"/>
@@ -1524,7 +1717,7 @@
     </row>
     <row r="23" spans="1:70">
       <c r="A23" s="8" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="8"/>
       <c r="C23" s="8"/>
@@ -1536,7 +1729,7 @@
         <v>6</v>
       </c>
       <c r="H23" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AD23" s="16">
         <v>8</v>
@@ -1549,7 +1742,7 @@
     </row>
     <row r="24" spans="1:70">
       <c r="A24" s="8" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B24" s="8"/>
       <c r="C24" s="8"/>
@@ -1561,7 +1754,7 @@
         <v>6</v>
       </c>
       <c r="H24" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I24" s="13"/>
       <c r="J24" s="13"/>
@@ -1580,7 +1773,7 @@
     </row>
     <row r="25" spans="1:70">
       <c r="A25" s="8" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B25" s="8"/>
       <c r="C25" s="8"/>
@@ -1592,7 +1785,7 @@
         <v>4</v>
       </c>
       <c r="H25" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="I25" s="15"/>
       <c r="J25" s="15"/>
@@ -1603,7 +1796,7 @@
     </row>
     <row r="26" spans="1:70">
       <c r="A26" s="8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B26" s="8"/>
       <c r="C26" s="8"/>
@@ -1621,17 +1814,23 @@
     </row>
     <row r="27" spans="1:70">
       <c r="A27" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B27" s="11"/>
       <c r="C27" s="11"/>
       <c r="D27" s="11"/>
       <c r="E27" s="10"/>
       <c r="F27" s="10"/>
+      <c r="G27">
+        <v>3</v>
+      </c>
+      <c r="I27" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="28" spans="1:70">
       <c r="A28" s="8" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B28" s="8"/>
       <c r="C28" s="8"/>
@@ -1642,12 +1841,12 @@
       </c>
       <c r="G28">
         <f>SUM(G15:G27)</f>
-        <v>5</v>
+        <v>12</v>
       </c>
     </row>
     <row r="29" spans="1:70">
       <c r="A29" s="2" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2"/>
       <c r="C29" s="2"/>
@@ -1656,15 +1855,33 @@
       <c r="F29" s="2"/>
       <c r="G29" s="2"/>
       <c r="H29" s="2"/>
-      <c r="I29" s="2"/>
-      <c r="J29" s="2"/>
-      <c r="K29" s="2"/>
-      <c r="L29" s="2"/>
-      <c r="M29" s="2"/>
-      <c r="N29" s="2"/>
-      <c r="O29" s="2"/>
-      <c r="P29" s="2"/>
-      <c r="Q29" s="2"/>
+      <c r="I29" s="2">
+        <v>1</v>
+      </c>
+      <c r="J29" s="2">
+        <v>2</v>
+      </c>
+      <c r="K29" s="2">
+        <v>3</v>
+      </c>
+      <c r="L29" s="2">
+        <v>4</v>
+      </c>
+      <c r="M29" s="2">
+        <v>5</v>
+      </c>
+      <c r="N29" s="2">
+        <v>6</v>
+      </c>
+      <c r="O29" s="2">
+        <v>7</v>
+      </c>
+      <c r="P29" s="2">
+        <v>8</v>
+      </c>
+      <c r="Q29" s="2">
+        <v>9</v>
+      </c>
       <c r="R29" s="2"/>
       <c r="S29" s="2"/>
       <c r="T29" s="2"/>
@@ -1721,7 +1938,7 @@
     </row>
     <row r="30" spans="1:70">
       <c r="A30" s="3" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
@@ -1733,13 +1950,13 @@
         <v>1</v>
       </c>
       <c r="H30" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I30" s="15"/>
     </row>
     <row r="31" spans="1:70">
       <c r="A31" s="5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B31" s="5"/>
       <c r="C31" s="5"/>
@@ -1751,7 +1968,7 @@
         <v>1</v>
       </c>
       <c r="H31" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="I31" s="13"/>
       <c r="J31" s="16">
@@ -1760,7 +1977,7 @@
     </row>
     <row r="32" spans="1:70">
       <c r="A32" s="3" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3"/>
@@ -1772,7 +1989,7 @@
         <v>1</v>
       </c>
       <c r="H32" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="J32" s="13"/>
       <c r="K32" s="16">
@@ -1781,7 +1998,7 @@
     </row>
     <row r="33" spans="1:65">
       <c r="A33" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
@@ -1793,7 +2010,7 @@
         <v>2</v>
       </c>
       <c r="H33" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="K33" s="13"/>
       <c r="L33" s="16">
@@ -1803,7 +2020,7 @@
     </row>
     <row r="34" spans="1:65">
       <c r="A34" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -1815,7 +2032,7 @@
         <v>1</v>
       </c>
       <c r="H34" s="12" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="N34" s="16">
         <v>4</v>
@@ -1823,7 +2040,7 @@
     </row>
     <row r="35" spans="1:65">
       <c r="A35" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B35" s="11"/>
       <c r="C35" s="11"/>
@@ -1833,7 +2050,7 @@
     </row>
     <row r="36" spans="1:65">
       <c r="A36" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B36" s="3"/>
       <c r="C36" s="3"/>
@@ -1848,7 +2065,7 @@
     </row>
     <row r="37" spans="1:65">
       <c r="A37" s="2" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B37" s="2"/>
       <c r="C37" s="2"/>
@@ -1917,7 +2134,7 @@
     </row>
     <row r="38" spans="1:65">
       <c r="A38" s="9" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B38" s="9"/>
       <c r="C38" s="9"/>
@@ -1932,7 +2149,7 @@
         <v>4</v>
       </c>
       <c r="H38" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="I38" s="14"/>
       <c r="J38" s="14"/>
@@ -1943,7 +2160,7 @@
     </row>
     <row r="39" spans="1:65">
       <c r="A39" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B39" s="4"/>
       <c r="C39" s="4"/>
@@ -1955,7 +2172,7 @@
         <v>6</v>
       </c>
       <c r="H39" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="O39" s="16">
         <v>1</v>
@@ -1968,7 +2185,7 @@
     </row>
     <row r="40" spans="1:65">
       <c r="A40" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B40" s="4"/>
       <c r="C40" s="4"/>
@@ -1980,7 +2197,7 @@
         <v>5</v>
       </c>
       <c r="H40" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="U40" s="16">
         <v>2</v>
@@ -1992,7 +2209,7 @@
     </row>
     <row r="41" spans="1:65">
       <c r="A41" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B41" s="4"/>
       <c r="C41" s="4"/>
@@ -2007,22 +2224,22 @@
         <v>6</v>
       </c>
       <c r="H41" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="I41" s="28"/>
-      <c r="J41" s="28"/>
-      <c r="K41" s="28"/>
-      <c r="L41" s="28"/>
-      <c r="M41" s="28"/>
-      <c r="N41" s="28"/>
-      <c r="O41" s="28"/>
-      <c r="P41" s="28"/>
-      <c r="Q41" s="28"/>
-      <c r="R41" s="28"/>
-      <c r="S41" s="28"/>
-      <c r="T41" s="28"/>
-      <c r="U41" s="28"/>
-      <c r="V41" s="28"/>
+        <v>47</v>
+      </c>
+      <c r="I41" s="23"/>
+      <c r="J41" s="23"/>
+      <c r="K41" s="23"/>
+      <c r="L41" s="23"/>
+      <c r="M41" s="23"/>
+      <c r="N41" s="23"/>
+      <c r="O41" s="23"/>
+      <c r="P41" s="23"/>
+      <c r="Q41" s="23"/>
+      <c r="R41" s="23"/>
+      <c r="S41" s="23"/>
+      <c r="T41" s="23"/>
+      <c r="U41" s="23"/>
+      <c r="V41" s="23"/>
       <c r="W41" s="10"/>
       <c r="X41" s="10"/>
       <c r="Y41" s="10"/>
@@ -2052,7 +2269,7 @@
     </row>
     <row r="42" spans="1:65">
       <c r="A42" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B42" s="4"/>
       <c r="C42" s="4"/>
@@ -2067,7 +2284,7 @@
         <v>3</v>
       </c>
       <c r="H42" s="14" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="I42" s="14"/>
       <c r="J42" s="14"/>
@@ -2109,7 +2326,7 @@
     </row>
     <row r="43" spans="1:65">
       <c r="A43" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B43" s="4"/>
       <c r="C43" s="4"/>
@@ -2121,10 +2338,10 @@
         <v>20</v>
       </c>
       <c r="H43" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z43" s="15" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="AA43" s="15"/>
       <c r="AB43" s="15"/>
@@ -2148,7 +2365,7 @@
     </row>
     <row r="44" spans="1:65">
       <c r="A44" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B44" s="4"/>
       <c r="C44" s="4"/>
@@ -2160,17 +2377,17 @@
         <v>3</v>
       </c>
       <c r="H44" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AT44" s="15" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="AU44" s="15"/>
       <c r="AV44" s="15"/>
     </row>
     <row r="45" spans="1:65">
       <c r="A45" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B45" s="4"/>
       <c r="C45" s="4"/>
@@ -2182,7 +2399,7 @@
         <v>3</v>
       </c>
       <c r="H45" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AT45" s="16">
         <v>6</v>
@@ -2192,7 +2409,7 @@
     </row>
     <row r="46" spans="1:65">
       <c r="A46" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B46" s="4"/>
       <c r="C46" s="4"/>
@@ -2204,10 +2421,10 @@
         <v>4</v>
       </c>
       <c r="H46" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AW46" s="15" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="AX46" s="15"/>
       <c r="AY46" s="15"/>
@@ -2215,7 +2432,7 @@
     </row>
     <row r="47" spans="1:65">
       <c r="A47" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B47" s="11"/>
       <c r="C47" s="11"/>
@@ -2225,7 +2442,7 @@
     </row>
     <row r="48" spans="1:65">
       <c r="A48" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B48" s="4"/>
       <c r="C48" s="4"/>
@@ -2241,7 +2458,7 @@
     </row>
     <row r="49" spans="1:69">
       <c r="A49" s="2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B49" s="2"/>
       <c r="C49" s="2"/>
@@ -2314,7 +2531,7 @@
     </row>
     <row r="50" spans="1:69">
       <c r="A50" s="4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B50" s="4"/>
       <c r="C50" s="4"/>
@@ -2329,13 +2546,13 @@
         <v>1</v>
       </c>
       <c r="H50" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="I50" s="7"/>
     </row>
     <row r="51" spans="1:69">
       <c r="A51" s="4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B51" s="4"/>
       <c r="C51" s="4"/>
@@ -2350,7 +2567,7 @@
         <v>2</v>
       </c>
       <c r="H51" s="7" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="J51" s="18">
         <v>1</v>
@@ -2359,7 +2576,7 @@
     </row>
     <row r="52" spans="1:69">
       <c r="A52" s="4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B52" s="4"/>
       <c r="C52" s="4"/>
@@ -2374,7 +2591,7 @@
         <v>4</v>
       </c>
       <c r="H52" s="14" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L52" s="19">
         <v>2</v>
@@ -2395,7 +2612,7 @@
     </row>
     <row r="53" spans="1:69">
       <c r="A53" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B53" s="4"/>
       <c r="C53" s="4"/>
@@ -2410,7 +2627,7 @@
         <v>0</v>
       </c>
       <c r="H53" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z53" s="16">
         <v>3</v>
@@ -2438,7 +2655,7 @@
     </row>
     <row r="54" spans="1:69">
       <c r="A54" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B54" s="4"/>
       <c r="C54" s="4"/>
@@ -2450,7 +2667,7 @@
         <v>23</v>
       </c>
       <c r="H54" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="Z54" s="16">
         <v>3</v>
@@ -2478,7 +2695,7 @@
     </row>
     <row r="55" spans="1:69">
       <c r="A55" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B55" s="4"/>
       <c r="C55" s="4"/>
@@ -2490,7 +2707,7 @@
         <v>7</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="AU55" s="16">
         <v>5</v>
@@ -2504,7 +2721,7 @@
     </row>
     <row r="56" spans="1:69">
       <c r="A56" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B56" s="4"/>
       <c r="C56" s="4"/>
@@ -2516,7 +2733,7 @@
         <v>5</v>
       </c>
       <c r="H56" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="BB56" s="16">
         <v>6</v>
@@ -2530,7 +2747,7 @@
     </row>
     <row r="57" spans="1:69">
       <c r="A57" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B57" s="4"/>
       <c r="C57" s="4"/>
@@ -2542,7 +2759,7 @@
         <v>2</v>
       </c>
       <c r="H57" s="12" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="BI57" s="16">
         <v>7</v>
@@ -2554,7 +2771,7 @@
     </row>
     <row r="58" spans="1:69">
       <c r="A58" s="11" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B58" s="11"/>
       <c r="C58" s="11"/>
@@ -2571,7 +2788,7 @@
     </row>
     <row r="59" spans="1:69">
       <c r="A59" s="9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="F59">
         <v>66</v>
@@ -2583,7 +2800,7 @@
     </row>
     <row r="60" spans="1:69">
       <c r="A60" s="2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B60" s="2"/>
       <c r="C60" s="2"/>
@@ -2655,28 +2872,28 @@
     </row>
     <row r="62" spans="1:69">
       <c r="A62" t="s">
+        <v>78</v>
+      </c>
+      <c r="B62" t="s">
+        <v>83</v>
+      </c>
+      <c r="D62" t="s">
         <v>79</v>
       </c>
-      <c r="B62" t="s">
+      <c r="E62" t="s">
+        <v>82</v>
+      </c>
+      <c r="G62" t="s">
+        <v>80</v>
+      </c>
+      <c r="H62" t="s">
+        <v>83</v>
+      </c>
+      <c r="J62" t="s">
+        <v>81</v>
+      </c>
+      <c r="K62" t="s">
         <v>84</v>
-      </c>
-      <c r="D62" t="s">
-        <v>80</v>
-      </c>
-      <c r="E62" t="s">
-        <v>83</v>
-      </c>
-      <c r="G62" t="s">
-        <v>81</v>
-      </c>
-      <c r="H62" t="s">
-        <v>84</v>
-      </c>
-      <c r="J62" t="s">
-        <v>82</v>
-      </c>
-      <c r="K62" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="63" spans="1:69">
@@ -2696,128 +2913,283 @@
     <row r="64" spans="1:69">
       <c r="B64" s="22"/>
     </row>
-    <row r="73" spans="1:5">
+    <row r="70" spans="1:16">
+      <c r="H70" s="42"/>
+      <c r="I70" s="43" t="s">
+        <v>92</v>
+      </c>
+      <c r="J70" s="43" t="s">
+        <v>93</v>
+      </c>
+      <c r="K70" s="44" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="71" spans="1:16">
+      <c r="H71" s="45" t="s">
+        <v>37</v>
+      </c>
+      <c r="I71" s="46">
+        <f>(F59+F48+F36+F28+F13)*100</f>
+        <v>21700</v>
+      </c>
+      <c r="J71" s="46">
+        <f>(G59+G48+G36+G28+G13)*100</f>
+        <v>4000</v>
+      </c>
+      <c r="K71" s="47">
+        <f>J71-I71</f>
+        <v>-17700</v>
+      </c>
+    </row>
+    <row r="72" spans="1:16" ht="16.3" thickBot="1">
+      <c r="H72" s="48" t="s">
+        <v>95</v>
+      </c>
+      <c r="I72" s="41">
+        <v>4800</v>
+      </c>
+      <c r="J72" s="41">
+        <f>SUM(C86:F86)</f>
+        <v>3800</v>
+      </c>
+      <c r="K72" s="49">
+        <f>J72-I72</f>
+        <v>-1000</v>
+      </c>
+    </row>
+    <row r="73" spans="1:16" ht="16.3" thickTop="1">
       <c r="A73" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="C73">
         <f>SUM(G13+G28+G36+G48+G59+A63+D63+G63+J63)</f>
-        <v>65</v>
+        <v>72</v>
       </c>
       <c r="D73" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="74" spans="1:5">
+        <v>85</v>
+      </c>
+      <c r="H73" s="34" t="s">
+        <v>24</v>
+      </c>
+      <c r="I73" s="50">
+        <f>I72+I71</f>
+        <v>26500</v>
+      </c>
+      <c r="J73" s="50">
+        <f t="shared" ref="J73:K73" si="0">J72+J71</f>
+        <v>7800</v>
+      </c>
+      <c r="K73" s="51">
+        <f t="shared" si="0"/>
+        <v>-18700</v>
+      </c>
+      <c r="P73" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="74" spans="1:16">
       <c r="C74" s="21">
         <f>C73*100</f>
-        <v>6500</v>
+        <v>7200</v>
       </c>
       <c r="D74" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="76" spans="1:5">
-      <c r="B76" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="76" spans="1:16">
+      <c r="B76" s="31" t="s">
+        <v>65</v>
+      </c>
+      <c r="C76" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="D76" s="32" t="s">
         <v>66</v>
       </c>
-      <c r="C76" t="s">
+      <c r="E76" s="32" t="s">
+        <v>64</v>
+      </c>
+      <c r="F76" s="33" t="s">
         <v>67</v>
       </c>
-      <c r="D76" t="s">
-        <v>65</v>
-      </c>
-      <c r="E76" t="s">
+    </row>
+    <row r="77" spans="1:16">
+      <c r="B77" s="34" t="s">
         <v>68</v>
       </c>
-    </row>
-    <row r="77" spans="1:5">
-      <c r="B77" t="s">
+      <c r="C77" s="30" t="s">
+        <v>78</v>
+      </c>
+      <c r="D77" s="30" t="s">
+        <v>75</v>
+      </c>
+      <c r="E77" s="30" t="s">
+        <v>76</v>
+      </c>
+      <c r="F77" s="35" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="78" spans="1:16" hidden="1">
+      <c r="B78" s="36" t="s">
         <v>69</v>
       </c>
-      <c r="C77" t="s">
-        <v>76</v>
-      </c>
-      <c r="D77" t="s">
-        <v>77</v>
-      </c>
-      <c r="E77" t="s">
-        <v>78</v>
-      </c>
-    </row>
-    <row r="78" spans="1:5">
-      <c r="B78" t="s">
+      <c r="C78" s="37"/>
+      <c r="D78" s="37">
+        <v>3</v>
+      </c>
+      <c r="E78" s="37">
+        <v>3</v>
+      </c>
+      <c r="F78" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="79" spans="1:16">
+      <c r="B79" s="36" t="s">
         <v>70</v>
       </c>
-      <c r="C78">
-        <v>3</v>
-      </c>
-      <c r="D78">
-        <v>3</v>
-      </c>
-      <c r="E78">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="79" spans="1:5">
-      <c r="A79" t="s">
+      <c r="C79" s="37">
+        <v>1</v>
+      </c>
+      <c r="D79" s="37">
+        <v>3</v>
+      </c>
+      <c r="E79" s="37">
+        <v>3</v>
+      </c>
+      <c r="F79" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="80" spans="1:16">
+      <c r="B80" s="36" t="s">
         <v>71</v>
       </c>
-      <c r="C79">
-        <v>3</v>
-      </c>
-      <c r="D79">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="80" spans="1:5">
-      <c r="A80" t="s">
+      <c r="C80" s="37">
+        <v>1</v>
+      </c>
+      <c r="D80" s="37">
+        <v>3</v>
+      </c>
+      <c r="E80" s="37">
+        <v>3</v>
+      </c>
+      <c r="F80" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="81" spans="2:6">
+      <c r="B81" s="36" t="s">
         <v>72</v>
       </c>
-      <c r="C80">
-        <v>3</v>
-      </c>
-      <c r="D80">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="81" spans="1:4">
-      <c r="A81" t="s">
+      <c r="C81" s="37">
+        <v>1</v>
+      </c>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37">
+        <v>3</v>
+      </c>
+      <c r="F81" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="82" spans="2:6">
+      <c r="B82" s="36" t="s">
         <v>73</v>
       </c>
-      <c r="D81">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4">
-      <c r="A82" t="s">
+      <c r="C82" s="37">
+        <v>1</v>
+      </c>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37">
+        <v>3</v>
+      </c>
+      <c r="F82" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="83" spans="2:6">
+      <c r="B83" s="36" t="s">
         <v>74</v>
       </c>
-      <c r="D82">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="83" spans="1:4">
-      <c r="A83" t="s">
-        <v>75</v>
-      </c>
-      <c r="C83">
-        <v>3</v>
-      </c>
-      <c r="D83">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4">
-      <c r="A84" t="s">
-        <v>54</v>
-      </c>
-      <c r="D84">
-        <v>3</v>
+      <c r="C83" s="37">
+        <v>1</v>
+      </c>
+      <c r="D83" s="37">
+        <v>3</v>
+      </c>
+      <c r="E83" s="37">
+        <v>3</v>
+      </c>
+      <c r="F83" s="38">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="84" spans="2:6" ht="16.3" thickBot="1">
+      <c r="B84" s="39" t="s">
+        <v>53</v>
+      </c>
+      <c r="C84" s="29">
+        <v>1</v>
+      </c>
+      <c r="D84" s="29"/>
+      <c r="E84" s="29">
+        <v>3</v>
+      </c>
+      <c r="F84" s="40"/>
+    </row>
+    <row r="85" spans="2:6" ht="16.3" thickTop="1">
+      <c r="B85" s="36" t="s">
+        <v>24</v>
+      </c>
+      <c r="C85" s="37">
+        <f>SUM(C79:C84)</f>
+        <v>6</v>
+      </c>
+      <c r="D85" s="37">
+        <f t="shared" ref="D85:F85" si="1">SUM(D79:D84)</f>
+        <v>9</v>
+      </c>
+      <c r="E85" s="37">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
+      <c r="F85" s="38">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="2:6">
+      <c r="B86" s="34" t="s">
+        <v>90</v>
+      </c>
+      <c r="C86" s="30">
+        <f>C85*100</f>
+        <v>600</v>
+      </c>
+      <c r="D86" s="30">
+        <f>D85*100</f>
+        <v>900</v>
+      </c>
+      <c r="E86" s="30">
+        <f t="shared" ref="E86:F86" si="2">E85*100</f>
+        <v>1800</v>
+      </c>
+      <c r="F86" s="35">
+        <f t="shared" si="2"/>
+        <v>500</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="14">
+    <mergeCell ref="A6:D6"/>
+    <mergeCell ref="A1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="A3:D3"/>
+    <mergeCell ref="A4:D4"/>
+    <mergeCell ref="A5:D5"/>
     <mergeCell ref="A12:D12"/>
     <mergeCell ref="A21:D21"/>
     <mergeCell ref="A7:D7"/>
@@ -2826,14 +3198,18 @@
     <mergeCell ref="A10:D10"/>
     <mergeCell ref="A11:D11"/>
     <mergeCell ref="A13:D13"/>
-    <mergeCell ref="A6:D6"/>
-    <mergeCell ref="A1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="A3:D3"/>
-    <mergeCell ref="A4:D4"/>
-    <mergeCell ref="A5:D5"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
+  <conditionalFormatting sqref="K71:K72">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K73">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="lessThan">
+      <formula>0</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
@@ -2847,44 +3223,44 @@
       <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.69921875" defaultRowHeight="15.6"/>
+  <sheetFormatPr defaultColWidth="10.7109375" defaultRowHeight="15.9"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="20"/>
       <c r="B1" s="20" t="s">
+        <v>65</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>66</v>
       </c>
-      <c r="C1" s="20" t="s">
+      <c r="D1" s="20" t="s">
+        <v>64</v>
+      </c>
+      <c r="E1" s="20" t="s">
         <v>67</v>
-      </c>
-      <c r="D1" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="E1" s="20" t="s">
-        <v>68</v>
       </c>
       <c r="F1" s="20"/>
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="20"/>
       <c r="B2" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C2" s="20" t="s">
+        <v>75</v>
+      </c>
+      <c r="D2" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="E2" s="20" t="s">
         <v>77</v>
-      </c>
-      <c r="E2" s="20" t="s">
-        <v>78</v>
       </c>
       <c r="F2" s="20"/>
     </row>
     <row r="3" spans="1:6">
       <c r="A3" s="20"/>
       <c r="B3" s="20" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3" s="20">
         <v>3</v>
@@ -2899,7 +3275,7 @@
     </row>
     <row r="4" spans="1:6">
       <c r="A4" s="20" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B4" s="20"/>
       <c r="C4" s="20">
@@ -2913,7 +3289,7 @@
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="20" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B5" s="20"/>
       <c r="C5" s="20">
@@ -2927,7 +3303,7 @@
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B6" s="20"/>
       <c r="C6" s="20">
@@ -2943,7 +3319,7 @@
     </row>
     <row r="7" spans="1:6">
       <c r="A7" s="20" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B7" s="20"/>
       <c r="C7" s="20"/>
@@ -2955,7 +3331,7 @@
     </row>
     <row r="8" spans="1:6">
       <c r="A8" s="20" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B8" s="20"/>
       <c r="C8" s="20">
@@ -2969,7 +3345,7 @@
     </row>
     <row r="9" spans="1:6">
       <c r="A9" s="20" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B9" s="20"/>
       <c r="C9" s="20"/>

</xml_diff>